<commit_message>
Nop bai lan 2 da chay full test suite
</commit_message>
<xml_diff>
--- a/assignment/tran-quang-lam/assignment-webui/Data Files/Excel files/dat-hang-va-thanh-toan.xlsx
+++ b/assignment/tran-quang-lam/assignment-webui/Data Files/Excel files/dat-hang-va-thanh-toan.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\katalon\assignment\tran-quang-lam\assignment-webui\Data Files\Excel files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C51F01BA-3EC2-4AEF-8835-3DB97A5D32C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A6A5A69-300F-4108-B9D0-596CDB45F82C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{CA38DB98-14BC-4EF2-9E95-EA58245DC1DD}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="41">
   <si>
     <t>name</t>
   </si>
@@ -152,16 +152,13 @@
     <t>quynhnguyen136@gmail.com</t>
   </si>
   <si>
-    <t>quydo937@gmail.com</t>
-  </si>
-  <si>
-    <t>quynhnguyen123</t>
-  </si>
-  <si>
     <t>quynhnguyen138@gmail.com</t>
   </si>
   <si>
-    <t>quynhnguyen141@gmail.com</t>
+    <t>quynhnguyen906@gmail.com</t>
+  </si>
+  <si>
+    <t>quynhnguyen901@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -554,7 +551,7 @@
   <dimension ref="A1:W6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -781,10 +778,10 @@
     </row>
     <row r="4" spans="1:23" x14ac:dyDescent="0.3">
       <c r="B4" s="1" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="C4" t="s">
-        <v>39</v>
+        <v>17</v>
       </c>
       <c r="Q4" t="s">
         <v>32</v>
@@ -813,7 +810,7 @@
         <v>16</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C5" t="s">
         <v>17</v>
@@ -866,7 +863,7 @@
         <v>16</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C6" t="s">
         <v>17</v>
@@ -937,9 +934,9 @@
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1" xr:uid="{130271B4-88A3-4EAB-9585-8F47C5662F10}"/>
     <hyperlink ref="B3" r:id="rId2" xr:uid="{40D5E1F6-18C9-4BEA-9EF1-6D85D74E9E48}"/>
-    <hyperlink ref="B4" r:id="rId3" xr:uid="{F25E054B-A900-4D8A-BA53-F3874A1AA83B}"/>
-    <hyperlink ref="B5" r:id="rId4" xr:uid="{B98E4E4B-AFA9-4261-AC72-EC2AE9F8AD10}"/>
-    <hyperlink ref="B6" r:id="rId5" xr:uid="{B41C9336-EC9C-4CFD-9A6E-79E964F8A893}"/>
+    <hyperlink ref="B5" r:id="rId3" xr:uid="{B98E4E4B-AFA9-4261-AC72-EC2AE9F8AD10}"/>
+    <hyperlink ref="B6" r:id="rId4" xr:uid="{43615EE5-54E0-4757-8B12-F24B2D5204D8}"/>
+    <hyperlink ref="B4" r:id="rId5" xr:uid="{A33CC133-601F-4952-8BE3-D903CC1BCFF8}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>